<commit_message>
adds ability for base capability
</commit_message>
<xml_diff>
--- a/files/example.xlsx
+++ b/files/example.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="64">
   <si>
     <t>Resource Registry Init</t>
   </si>
@@ -215,6 +215,9 @@
   </si>
   <si>
     <t>camera</t>
+  </si>
+  <si>
+    <t>DC_Base</t>
   </si>
 </sst>
 </file>
@@ -290,8 +293,20 @@
     <dxf>
       <font>
         <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
       </font>
-      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -308,20 +323,8 @@
     <dxf>
       <font>
         <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
       </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -465,9 +468,9 @@
     <tableColumn id="19" name="connection-port" dataDxfId="8"/>
     <tableColumn id="23" name="location-uuid" dataDxfId="7"/>
     <tableColumn id="24" name="aasx-filter-substring" dataDxfId="6"/>
-    <tableColumn id="20" name="DC_Dummy" dataDxfId="5"/>
-    <tableColumn id="21" name="DC_Shell" dataDxfId="4"/>
-    <tableColumn id="22" name="DC_Dummy2" dataDxfId="3"/>
+    <tableColumn id="25" name="DC_Base" dataDxfId="0"/>
+    <tableColumn id="21" name="DC_Shell" dataDxfId="5"/>
+    <tableColumn id="22" name="DC_Dummy2" dataDxfId="4"/>
     <tableColumn id="15" name="DC_Docker"/>
     <tableColumn id="16" name="DC_Transferapp"/>
     <tableColumn id="17" name="DC_Swarm"/>
@@ -478,11 +481,11 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="TLOCATIONS" displayName="TLOCATIONS" ref="A1:B5" totalsRowShown="0" dataDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="TLOCATIONS" displayName="TLOCATIONS" ref="A1:B5" totalsRowShown="0" dataDxfId="3">
   <autoFilter ref="A1:B5"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="UUID" dataDxfId="1"/>
-    <tableColumn id="2" name="Name" dataDxfId="0"/>
+    <tableColumn id="1" name="UUID" dataDxfId="2"/>
+    <tableColumn id="2" name="Name" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -894,10 +897,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X16"/>
+  <dimension ref="A1:Y16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+      <selection activeCell="R1" sqref="R1:Y1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -918,18 +921,18 @@
     <col min="14" max="14" width="22.7109375" style="3" customWidth="1"/>
     <col min="15" max="15" width="25.5703125" style="3" customWidth="1"/>
     <col min="16" max="16" width="36" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="36" style="3" customWidth="1"/>
-    <col min="18" max="18" width="12.85546875" style="3" customWidth="1"/>
+    <col min="17" max="18" width="36" style="3" customWidth="1"/>
     <col min="19" max="19" width="11.28515625" style="3" customWidth="1"/>
     <col min="20" max="20" width="14.42578125" style="3" customWidth="1"/>
     <col min="21" max="21" width="12.42578125" style="3" customWidth="1"/>
     <col min="22" max="22" width="16.5703125" style="3" customWidth="1"/>
     <col min="23" max="23" width="12.140625" style="3" customWidth="1"/>
     <col min="24" max="24" width="9.42578125" style="3" customWidth="1"/>
+    <col min="25" max="25" width="9.28515625" style="3" customWidth="1"/>
     <col min="1028" max="1030" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
@@ -982,7 +985,7 @@
         <v>61</v>
       </c>
       <c r="R1" s="5" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="S1" s="5" t="s">
         <v>44</v>
@@ -1002,8 +1005,11 @@
       <c r="X1" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:24" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Y1" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>21</v>
       </c>
@@ -1051,7 +1057,9 @@
       <c r="Q2" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="R2" s="5"/>
+      <c r="R2" s="5" t="s">
+        <v>30</v>
+      </c>
       <c r="S2" s="5" t="s">
         <v>27</v>
       </c>
@@ -1070,8 +1078,11 @@
       <c r="X2" s="5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:24" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Y2" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>32</v>
       </c>
@@ -1115,7 +1126,9 @@
         <v>51</v>
       </c>
       <c r="Q3" s="5"/>
-      <c r="R3" s="5"/>
+      <c r="R3" s="5" t="s">
+        <v>30</v>
+      </c>
       <c r="S3" s="5" t="s">
         <v>27</v>
       </c>
@@ -1134,8 +1147,11 @@
       <c r="X3" s="5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="4" spans="1:24" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Y3" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>57</v>
       </c>
@@ -1181,7 +1197,9 @@
       <c r="Q4" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="R4" s="5"/>
+      <c r="R4" s="5" t="s">
+        <v>30</v>
+      </c>
       <c r="S4" s="5" t="s">
         <v>27</v>
       </c>
@@ -1200,8 +1218,11 @@
       <c r="X4" s="5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="5" spans="1:24" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Y4" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -1226,8 +1247,9 @@
       <c r="V5" s="5"/>
       <c r="W5" s="5"/>
       <c r="X5" s="5"/>
-    </row>
-    <row r="6" spans="1:24" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Y5" s="5"/>
+    </row>
+    <row r="6" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -1252,8 +1274,9 @@
       <c r="V6" s="5"/>
       <c r="W6" s="5"/>
       <c r="X6" s="5"/>
-    </row>
-    <row r="7" spans="1:24" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Y6" s="5"/>
+    </row>
+    <row r="7" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -1278,8 +1301,9 @@
       <c r="V7" s="5"/>
       <c r="W7" s="5"/>
       <c r="X7" s="5"/>
-    </row>
-    <row r="8" spans="1:24" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Y7" s="5"/>
+    </row>
+    <row r="8" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -1304,8 +1328,9 @@
       <c r="V8" s="5"/>
       <c r="W8" s="5"/>
       <c r="X8" s="5"/>
-    </row>
-    <row r="9" spans="1:24" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Y8" s="5"/>
+    </row>
+    <row r="9" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -1330,8 +1355,9 @@
       <c r="V9" s="5"/>
       <c r="W9" s="5"/>
       <c r="X9" s="5"/>
-    </row>
-    <row r="10" spans="1:24" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Y9" s="5"/>
+    </row>
+    <row r="10" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -1356,8 +1382,9 @@
       <c r="V10" s="5"/>
       <c r="W10" s="5"/>
       <c r="X10" s="5"/>
-    </row>
-    <row r="11" spans="1:24" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Y10" s="5"/>
+    </row>
+    <row r="11" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -1382,8 +1409,9 @@
       <c r="V11" s="5"/>
       <c r="W11" s="5"/>
       <c r="X11" s="5"/>
-    </row>
-    <row r="12" spans="1:24" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Y11" s="5"/>
+    </row>
+    <row r="12" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -1408,8 +1436,9 @@
       <c r="V12" s="5"/>
       <c r="W12" s="5"/>
       <c r="X12" s="5"/>
-    </row>
-    <row r="13" spans="1:24" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Y12" s="5"/>
+    </row>
+    <row r="13" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -1434,8 +1463,9 @@
       <c r="V13" s="5"/>
       <c r="W13" s="5"/>
       <c r="X13" s="5"/>
-    </row>
-    <row r="14" spans="1:24" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Y13" s="5"/>
+    </row>
+    <row r="14" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -1460,8 +1490,9 @@
       <c r="V14" s="5"/>
       <c r="W14" s="5"/>
       <c r="X14" s="5"/>
-    </row>
-    <row r="15" spans="1:24" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Y14" s="5"/>
+    </row>
+    <row r="15" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -1486,8 +1517,9 @@
       <c r="V15" s="5"/>
       <c r="W15" s="5"/>
       <c r="X15" s="5"/>
-    </row>
-    <row r="16" spans="1:24" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Y15" s="5"/>
+    </row>
+    <row r="16" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>

</xml_diff>

<commit_message>
adds service group handling
</commit_message>
<xml_diff>
--- a/files/example.xlsx
+++ b/files/example.xlsx
@@ -15,6 +15,7 @@
     <sheet name="INFO" sheetId="1" r:id="rId1"/>
     <sheet name="DEVICES" sheetId="2" r:id="rId2"/>
     <sheet name="LOCATIONS" sheetId="3" r:id="rId3"/>
+    <sheet name="SERVICE_GROUPS" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="68">
   <si>
     <t>Resource Registry Init</t>
   </si>
@@ -160,15 +161,9 @@
     <t>connection-port</t>
   </si>
   <si>
-    <t>DC_Shell</t>
-  </si>
-  <si>
     <t>DC_Dummy</t>
   </si>
   <si>
-    <t>DC_Dummy2</t>
-  </si>
-  <si>
     <t>SLM Demo</t>
   </si>
   <si>
@@ -218,6 +213,24 @@
   </si>
   <si>
     <t>DC_Base</t>
+  </si>
+  <si>
+    <t>Griff in die Kiste</t>
+  </si>
+  <si>
+    <t>IPA Cubes</t>
+  </si>
+  <si>
+    <t>Test Group</t>
+  </si>
+  <si>
+    <t>fcf12e8d-2214-4ab0-b148-16f5c940e4cf</t>
+  </si>
+  <si>
+    <t>59623727-3784-4864-9260-9008bc79d5d8</t>
+  </si>
+  <si>
+    <t>70bfdfb9-23b2-44d0-a90c-a04d5e05a41c</t>
   </si>
 </sst>
 </file>
@@ -289,7 +302,7 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="12">
     <dxf>
       <font>
         <b val="0"/>
@@ -307,6 +320,24 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -416,24 +447,6 @@
       </font>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -448,9 +461,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TDEVICES" displayName="TDEVICES" ref="A1:X15" totalsRowShown="0">
-  <autoFilter ref="A1:X15"/>
-  <tableColumns count="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TDEVICES" displayName="TDEVICES" ref="A1:W5" totalsRowShown="0">
+  <autoFilter ref="A1:W5"/>
+  <tableColumns count="23">
     <tableColumn id="1" name="Device"/>
     <tableColumn id="2" name="OS"/>
     <tableColumn id="3" name="user"/>
@@ -464,30 +477,40 @@
     <tableColumn id="11" name="eth1 IP"/>
     <tableColumn id="12" name="is_resource"/>
     <tableColumn id="13" name="UUID"/>
-    <tableColumn id="14" name="connection-type" dataDxfId="9"/>
-    <tableColumn id="19" name="connection-port" dataDxfId="8"/>
-    <tableColumn id="23" name="location-uuid" dataDxfId="7"/>
-    <tableColumn id="24" name="aasx-filter-substring" dataDxfId="6"/>
-    <tableColumn id="25" name="DC_Base" dataDxfId="0"/>
-    <tableColumn id="21" name="DC_Shell" dataDxfId="5"/>
-    <tableColumn id="22" name="DC_Dummy2" dataDxfId="4"/>
+    <tableColumn id="14" name="connection-type" dataDxfId="11"/>
+    <tableColumn id="19" name="connection-port" dataDxfId="10"/>
+    <tableColumn id="23" name="location-uuid" dataDxfId="9"/>
+    <tableColumn id="24" name="aasx-filter-substring" dataDxfId="8"/>
+    <tableColumn id="25" name="DC_Base" dataDxfId="7"/>
     <tableColumn id="15" name="DC_Docker"/>
     <tableColumn id="16" name="DC_Transferapp"/>
     <tableColumn id="17" name="DC_Swarm"/>
     <tableColumn id="18" name="DC_K3S"/>
+    <tableColumn id="20" name="DC_Dummy" dataDxfId="0"/>
   </tableColumns>
-  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="TLOCATIONS" displayName="TLOCATIONS" ref="A1:B5" totalsRowShown="0" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="TLOCATIONS" displayName="TLOCATIONS" ref="A1:B5" totalsRowShown="0" dataDxfId="6">
   <autoFilter ref="A1:B5"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="UUID" dataDxfId="5"/>
+    <tableColumn id="2" name="Name" dataDxfId="4"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="TLOCATIONS4" displayName="TLOCATIONS4" ref="A1:B4" totalsRowShown="0" dataDxfId="3">
+  <autoFilter ref="A1:B4"/>
   <tableColumns count="2">
     <tableColumn id="1" name="UUID" dataDxfId="2"/>
     <tableColumn id="2" name="Name" dataDxfId="1"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -897,10 +920,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y16"/>
+  <dimension ref="A1:W6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1:Y1048576"/>
+      <selection activeCell="S3" sqref="S3:S4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -921,18 +944,17 @@
     <col min="14" max="14" width="22.7109375" style="3" customWidth="1"/>
     <col min="15" max="15" width="25.5703125" style="3" customWidth="1"/>
     <col min="16" max="16" width="36" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="36" style="3" customWidth="1"/>
-    <col min="19" max="19" width="11.28515625" style="3" customWidth="1"/>
-    <col min="20" max="20" width="14.42578125" style="3" customWidth="1"/>
-    <col min="21" max="21" width="12.42578125" style="3" customWidth="1"/>
-    <col min="22" max="22" width="16.5703125" style="3" customWidth="1"/>
-    <col min="23" max="23" width="12.140625" style="3" customWidth="1"/>
-    <col min="24" max="24" width="9.42578125" style="3" customWidth="1"/>
-    <col min="25" max="25" width="9.28515625" style="3" customWidth="1"/>
-    <col min="1028" max="1030" width="9.140625" customWidth="1"/>
+    <col min="17" max="17" width="36" style="3" customWidth="1"/>
+    <col min="18" max="18" width="11.5703125" style="3" customWidth="1"/>
+    <col min="19" max="19" width="12.42578125" style="3" customWidth="1"/>
+    <col min="20" max="20" width="16.5703125" style="3" customWidth="1"/>
+    <col min="21" max="21" width="12.140625" style="3" customWidth="1"/>
+    <col min="22" max="22" width="9.42578125" style="3" customWidth="1"/>
+    <col min="23" max="23" width="13.42578125" style="3" customWidth="1"/>
+    <col min="1026" max="1028" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
@@ -979,37 +1001,31 @@
         <v>43</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="Q1" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="R1" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="R1" s="5" t="s">
-        <v>63</v>
-      </c>
       <c r="S1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="T1" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="U1" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="V1" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="W1" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="X1" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="Y1" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>21</v>
       </c>
@@ -1052,13 +1068,13 @@
         <v>22</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="R2" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="S2" s="5" t="s">
         <v>27</v>
@@ -1075,14 +1091,8 @@
       <c r="W2" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="X2" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y2" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>32</v>
       </c>
@@ -1123,20 +1133,20 @@
         <v>22</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="Q3" s="5"/>
       <c r="R3" s="5" t="s">
         <v>30</v>
       </c>
       <c r="S3" s="5" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="T3" s="5" t="s">
         <v>27</v>
       </c>
       <c r="U3" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="V3" s="5" t="s">
         <v>27</v>
@@ -1144,16 +1154,10 @@
       <c r="W3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="X3" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y3" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>33</v>
@@ -1165,7 +1169,7 @@
         <v>35</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
@@ -1173,7 +1177,7 @@
         <v>37</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="J4" s="5" t="s">
         <v>39</v>
@@ -1183,7 +1187,7 @@
         <v>30</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="N4" s="5" t="s">
         <v>42</v>
@@ -1192,22 +1196,22 @@
         <v>22</v>
       </c>
       <c r="P4" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="Q4" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="R4" s="5" t="s">
         <v>30</v>
       </c>
       <c r="S4" s="5" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="T4" s="5" t="s">
         <v>27</v>
       </c>
       <c r="U4" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="V4" s="5" t="s">
         <v>27</v>
@@ -1215,14 +1219,8 @@
       <c r="W4" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="X4" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y4" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -1246,14 +1244,12 @@
       <c r="U5" s="5"/>
       <c r="V5" s="5"/>
       <c r="W5" s="5"/>
-      <c r="X5" s="5"/>
-      <c r="Y5" s="5"/>
-    </row>
-    <row r="6" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
-      <c r="D6" s="7"/>
+      <c r="D6" s="6"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
@@ -1261,276 +1257,6 @@
       <c r="I6" s="6"/>
       <c r="J6" s="5"/>
       <c r="K6" s="6"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
-      <c r="P6" s="5"/>
-      <c r="Q6" s="5"/>
-      <c r="R6" s="5"/>
-      <c r="S6" s="5"/>
-      <c r="T6" s="5"/>
-      <c r="U6" s="5"/>
-      <c r="V6" s="5"/>
-      <c r="W6" s="5"/>
-      <c r="X6" s="5"/>
-      <c r="Y6" s="5"/>
-    </row>
-    <row r="7" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
-      <c r="P7" s="5"/>
-      <c r="Q7" s="5"/>
-      <c r="R7" s="5"/>
-      <c r="S7" s="5"/>
-      <c r="T7" s="5"/>
-      <c r="U7" s="5"/>
-      <c r="V7" s="5"/>
-      <c r="W7" s="5"/>
-      <c r="X7" s="5"/>
-      <c r="Y7" s="5"/>
-    </row>
-    <row r="8" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="5"/>
-      <c r="Q8" s="5"/>
-      <c r="R8" s="5"/>
-      <c r="S8" s="5"/>
-      <c r="T8" s="5"/>
-      <c r="U8" s="5"/>
-      <c r="V8" s="5"/>
-      <c r="W8" s="5"/>
-      <c r="X8" s="5"/>
-      <c r="Y8" s="5"/>
-    </row>
-    <row r="9" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="5"/>
-      <c r="P9" s="5"/>
-      <c r="Q9" s="5"/>
-      <c r="R9" s="5"/>
-      <c r="S9" s="5"/>
-      <c r="T9" s="5"/>
-      <c r="U9" s="5"/>
-      <c r="V9" s="5"/>
-      <c r="W9" s="5"/>
-      <c r="X9" s="5"/>
-      <c r="Y9" s="5"/>
-    </row>
-    <row r="10" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
-      <c r="P10" s="5"/>
-      <c r="Q10" s="5"/>
-      <c r="R10" s="5"/>
-      <c r="S10" s="5"/>
-      <c r="T10" s="5"/>
-      <c r="U10" s="5"/>
-      <c r="V10" s="5"/>
-      <c r="W10" s="5"/>
-      <c r="X10" s="5"/>
-      <c r="Y10" s="5"/>
-    </row>
-    <row r="11" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
-      <c r="O11" s="5"/>
-      <c r="P11" s="5"/>
-      <c r="Q11" s="5"/>
-      <c r="R11" s="5"/>
-      <c r="S11" s="5"/>
-      <c r="T11" s="5"/>
-      <c r="U11" s="5"/>
-      <c r="V11" s="5"/>
-      <c r="W11" s="5"/>
-      <c r="X11" s="5"/>
-      <c r="Y11" s="5"/>
-    </row>
-    <row r="12" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
-      <c r="P12" s="5"/>
-      <c r="Q12" s="5"/>
-      <c r="R12" s="5"/>
-      <c r="S12" s="5"/>
-      <c r="T12" s="5"/>
-      <c r="U12" s="5"/>
-      <c r="V12" s="5"/>
-      <c r="W12" s="5"/>
-      <c r="X12" s="5"/>
-      <c r="Y12" s="5"/>
-    </row>
-    <row r="13" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="5"/>
-      <c r="O13" s="5"/>
-      <c r="P13" s="5"/>
-      <c r="Q13" s="5"/>
-      <c r="R13" s="5"/>
-      <c r="S13" s="5"/>
-      <c r="T13" s="5"/>
-      <c r="U13" s="5"/>
-      <c r="V13" s="5"/>
-      <c r="W13" s="5"/>
-      <c r="X13" s="5"/>
-      <c r="Y13" s="5"/>
-    </row>
-    <row r="14" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
-      <c r="O14" s="5"/>
-      <c r="P14" s="5"/>
-      <c r="Q14" s="5"/>
-      <c r="R14" s="5"/>
-      <c r="S14" s="5"/>
-      <c r="T14" s="5"/>
-      <c r="U14" s="5"/>
-      <c r="V14" s="5"/>
-      <c r="W14" s="5"/>
-      <c r="X14" s="5"/>
-      <c r="Y14" s="5"/>
-    </row>
-    <row r="15" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
-      <c r="N15" s="5"/>
-      <c r="O15" s="5"/>
-      <c r="P15" s="5"/>
-      <c r="Q15" s="5"/>
-      <c r="R15" s="5"/>
-      <c r="S15" s="5"/>
-      <c r="T15" s="5"/>
-      <c r="U15" s="5"/>
-      <c r="V15" s="5"/>
-      <c r="W15" s="5"/>
-      <c r="X15" s="5"/>
-      <c r="Y15" s="5"/>
-    </row>
-    <row r="16" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -1540,7 +1266,7 @@
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>LOCATIONS!$A$2:$A$5</xm:f>
@@ -1558,7 +1284,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection sqref="A1:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1572,39 +1298,94 @@
         <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
         <v>53</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>54</v>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
allows to skip capability install
</commit_message>
<xml_diff>
--- a/files/example.xlsx
+++ b/files/example.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="69">
   <si>
     <t>Resource Registry Init</t>
   </si>
@@ -231,6 +231,9 @@
   </si>
   <si>
     <t>70bfdfb9-23b2-44d0-a90c-a04d5e05a41c</t>
+  </si>
+  <si>
+    <t>skip</t>
   </si>
 </sst>
 </file>
@@ -306,20 +309,8 @@
     <dxf>
       <font>
         <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
       </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -354,8 +345,20 @@
     <dxf>
       <font>
         <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
       </font>
-      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -486,29 +489,29 @@
     <tableColumn id="16" name="DC_Transferapp"/>
     <tableColumn id="17" name="DC_Swarm"/>
     <tableColumn id="18" name="DC_K3S"/>
-    <tableColumn id="20" name="DC_Dummy" dataDxfId="0"/>
+    <tableColumn id="20" name="DC_Dummy" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="TLOCATIONS" displayName="TLOCATIONS" ref="A1:B5" totalsRowShown="0" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="TLOCATIONS" displayName="TLOCATIONS" ref="A1:B5" totalsRowShown="0" dataDxfId="5">
   <autoFilter ref="A1:B5"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="UUID" dataDxfId="5"/>
-    <tableColumn id="2" name="Name" dataDxfId="4"/>
+    <tableColumn id="1" name="UUID" dataDxfId="4"/>
+    <tableColumn id="2" name="Name" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="TLOCATIONS4" displayName="TLOCATIONS4" ref="A1:B4" totalsRowShown="0" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="TLOCATIONS4" displayName="TLOCATIONS4" ref="A1:B4" totalsRowShown="0" dataDxfId="2">
   <autoFilter ref="A1:B4"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="UUID" dataDxfId="2"/>
-    <tableColumn id="2" name="Name" dataDxfId="1"/>
+    <tableColumn id="1" name="UUID" dataDxfId="1"/>
+    <tableColumn id="2" name="Name" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -923,7 +926,7 @@
   <dimension ref="A1:W6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S3" sqref="S3:S4"/>
+      <selection activeCell="R3" sqref="R3:R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1140,7 +1143,7 @@
         <v>30</v>
       </c>
       <c r="S3" s="5" t="s">
-        <v>30</v>
+        <v>68</v>
       </c>
       <c r="T3" s="5" t="s">
         <v>27</v>
@@ -1205,7 +1208,7 @@
         <v>30</v>
       </c>
       <c r="S4" s="5" t="s">
-        <v>30</v>
+        <v>68</v>
       </c>
       <c r="T4" s="5" t="s">
         <v>27</v>

</xml_diff>